<commit_message>
Resolve alpha diversity summary stat to sample type.
</commit_message>
<xml_diff>
--- a/data/aldex2_ancom_h_v_c_output.xlsx
+++ b/data/aldex2_ancom_h_v_c_output.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/zlmg2b_umsystem_edu/Documents/Projects/current/16S/220211_Cat_Asthma/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D89E74B7-81F8-604F-99B2-3757FFD451DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{D89E74B7-81F8-604F-99B2-3757FFD451DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8B84E91-C065-3D42-A4B5-55D830DD3DD6}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aldex2_ancom_h_v_c_output" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1113,10 +1113,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1471,11 +1471,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1485,54 +1485,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -6997,6 +6997,16 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K158" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1" showButton="0"/>
+    <filterColumn colId="2" showButton="0"/>
+    <filterColumn colId="3" showButton="0"/>
+    <filterColumn colId="4" showButton="0"/>
+    <filterColumn colId="6" showButton="0"/>
+    <filterColumn colId="7" showButton="0"/>
+    <filterColumn colId="8" showButton="0"/>
+    <filterColumn colId="9" showButton="0"/>
+  </autoFilter>
   <mergeCells count="3">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>

</xml_diff>